<commit_message>
Audit table in excel finished
</commit_message>
<xml_diff>
--- a/Audit Table.xlsx
+++ b/Audit Table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VICTUS\Documents\GitHub\sql-quality-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46251E97-6254-4E2D-9E52-B8B565BFA9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B1014D-2A2E-4053-934F-5985FCA4176C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3C1F016C-EBC1-4B48-98C7-798CC0259E45}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="173">
   <si>
     <t>Audit_id</t>
   </si>
@@ -426,6 +427,135 @@
   </si>
   <si>
     <t>Rework</t>
+  </si>
+  <si>
+    <t>Big process mistake</t>
+  </si>
+  <si>
+    <t>No error found</t>
+  </si>
+  <si>
+    <t>No mistakes</t>
+  </si>
+  <si>
+    <t>Typo found</t>
+  </si>
+  <si>
+    <t>Incorrect text</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Corrections 5.4, 6.7 and 8.9 needed</t>
+  </si>
+  <si>
+    <t>Incorrect process, engineering ticket needed</t>
+  </si>
+  <si>
+    <t>Pretty good job, but some incorrect fields</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Major process deviation detected</t>
+  </si>
+  <si>
+    <t>No discrepancies observed</t>
+  </si>
+  <si>
+    <t>Spelling error identified in documentation</t>
+  </si>
+  <si>
+    <t>Incorrect wording in report section</t>
+  </si>
+  <si>
+    <t>Incomplete comment; clarification required</t>
+  </si>
+  <si>
+    <t>Corrections to sections 3.2, 4.1 and 7.5 required</t>
+  </si>
+  <si>
+    <t>Non-compliant workflow used, follow-up ticket required</t>
+  </si>
+  <si>
+    <t>Overall acceptable, but several fields require correction</t>
+  </si>
+  <si>
+    <t>Significant control failure in approval step</t>
+  </si>
+  <si>
+    <t>Minor data-entry errors present</t>
+  </si>
+  <si>
+    <t>Formatting inconsistencies throughout document</t>
+  </si>
+  <si>
+    <t>Missing mandatory reference or attachment</t>
+  </si>
+  <si>
+    <t>Evidence incomplete; additional support needed</t>
+  </si>
+  <si>
+    <t>Key requirement not implemented as specified</t>
+  </si>
+  <si>
+    <t>Procedure followed, but documentation missing details</t>
+  </si>
+  <si>
+    <t>Metrics calculated using incorrect method</t>
+  </si>
+  <si>
+    <t>Observation withdrawn after re-check; no issue found</t>
+  </si>
+  <si>
+    <t>No issues identified</t>
+  </si>
+  <si>
+    <t>Rework  need</t>
+  </si>
+  <si>
+    <t>Minor error in data-entry</t>
+  </si>
+  <si>
+    <t>Non critical documentation missing</t>
+  </si>
+  <si>
+    <t>Incorrect format for approval</t>
+  </si>
+  <si>
+    <t>Wrong results as decimals not used</t>
+  </si>
+  <si>
+    <t>Major critical issue</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>No need</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorrect format </t>
+  </si>
+  <si>
+    <t>Incorrect process followed</t>
+  </si>
+  <si>
+    <t>No rework needed</t>
+  </si>
+  <si>
+    <t>Very different results from expected</t>
+  </si>
+  <si>
+    <t>Good job, no errors</t>
+  </si>
+  <si>
+    <t>Nothing wrong found</t>
+  </si>
+  <si>
+    <t>missing email</t>
   </si>
 </sst>
 </file>
@@ -798,20 +928,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34B2119-BDFE-4C7F-8CFA-7E93CF3210B0}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" hidden="1"/>
+    <col min="14" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -871,6 +1005,9 @@
       <c r="F2" t="s">
         <v>119</v>
       </c>
+      <c r="G2" t="s">
+        <v>130</v>
+      </c>
       <c r="H2">
         <v>8</v>
       </c>
@@ -880,9 +1017,11 @@
       <c r="J2">
         <v>0</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
       <c r="L2" s="1">
-        <f ca="1">NOW()-35.4</f>
-        <v>45980.465575925926</v>
+        <v>45980.001782407409</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -904,6 +1043,9 @@
       <c r="F3" t="s">
         <v>119</v>
       </c>
+      <c r="G3" t="s">
+        <v>131</v>
+      </c>
       <c r="H3">
         <v>0</v>
       </c>
@@ -913,9 +1055,11 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L2:L45" ca="1" si="0">NOW()-35</f>
-        <v>45980.865575925927</v>
+        <v>45980.004074074073</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -937,6 +1081,9 @@
       <c r="F4" t="s">
         <v>117</v>
       </c>
+      <c r="G4" t="s">
+        <v>132</v>
+      </c>
       <c r="H4">
         <v>0</v>
       </c>
@@ -946,9 +1093,11 @@
       <c r="J4">
         <v>0</v>
       </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="L4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.054373367821</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -970,6 +1119,9 @@
       <c r="F5" t="s">
         <v>120</v>
       </c>
+      <c r="G5" t="s">
+        <v>133</v>
+      </c>
       <c r="H5">
         <v>1</v>
       </c>
@@ -979,9 +1131,11 @@
       <c r="J5">
         <v>0</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
       <c r="L5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.062879867648</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1003,6 +1157,9 @@
       <c r="F6" t="s">
         <v>120</v>
       </c>
+      <c r="G6" t="s">
+        <v>134</v>
+      </c>
       <c r="H6">
         <v>2</v>
       </c>
@@ -1012,9 +1169,11 @@
       <c r="J6">
         <v>0</v>
       </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
       <c r="L6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.065445785767</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1036,6 +1195,9 @@
       <c r="F7" t="s">
         <v>118</v>
       </c>
+      <c r="G7" t="s">
+        <v>135</v>
+      </c>
       <c r="H7">
         <v>0</v>
       </c>
@@ -1045,9 +1207,11 @@
       <c r="J7">
         <v>0</v>
       </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
       <c r="L7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.068372531576</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1069,6 +1233,9 @@
       <c r="F8" t="s">
         <v>118</v>
       </c>
+      <c r="G8" t="s">
+        <v>136</v>
+      </c>
       <c r="H8">
         <v>9</v>
       </c>
@@ -1078,9 +1245,11 @@
       <c r="J8">
         <v>1</v>
       </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
       <c r="L8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.096311333931</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1102,6 +1271,9 @@
       <c r="F9" t="s">
         <v>122</v>
       </c>
+      <c r="G9" t="s">
+        <v>137</v>
+      </c>
       <c r="H9">
         <v>6</v>
       </c>
@@ -1111,9 +1283,11 @@
       <c r="J9">
         <v>0</v>
       </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
       <c r="L9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.140794824096</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1135,6 +1309,9 @@
       <c r="F10" t="s">
         <v>119</v>
       </c>
+      <c r="G10" t="s">
+        <v>138</v>
+      </c>
       <c r="H10">
         <v>4</v>
       </c>
@@ -1144,9 +1321,11 @@
       <c r="J10">
         <v>0</v>
       </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
       <c r="L10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.156893410371</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1168,6 +1347,9 @@
       <c r="F11" t="s">
         <v>119</v>
       </c>
+      <c r="G11" t="s">
+        <v>139</v>
+      </c>
       <c r="H11">
         <v>0</v>
       </c>
@@ -1177,9 +1359,11 @@
       <c r="J11">
         <v>0</v>
       </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
       <c r="L11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.210053623603</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1201,6 +1385,9 @@
       <c r="F12" t="s">
         <v>119</v>
       </c>
+      <c r="G12" t="s">
+        <v>149</v>
+      </c>
       <c r="H12">
         <v>3</v>
       </c>
@@ -1210,9 +1397,11 @@
       <c r="J12">
         <v>0</v>
       </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
       <c r="L12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.22066285491</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1234,6 +1423,9 @@
       <c r="F13" t="s">
         <v>117</v>
       </c>
+      <c r="G13" t="s">
+        <v>139</v>
+      </c>
       <c r="H13">
         <v>2</v>
       </c>
@@ -1243,9 +1435,11 @@
       <c r="J13">
         <v>0</v>
       </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
       <c r="L13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.223891000482</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1267,6 +1461,9 @@
       <c r="F14" t="s">
         <v>117</v>
       </c>
+      <c r="G14" t="s">
+        <v>157</v>
+      </c>
       <c r="H14">
         <v>0</v>
       </c>
@@ -1276,9 +1473,11 @@
       <c r="J14">
         <v>0</v>
       </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
       <c r="L14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.228297097412</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1300,6 +1499,9 @@
       <c r="F15" t="s">
         <v>118</v>
       </c>
+      <c r="G15" t="s">
+        <v>141</v>
+      </c>
       <c r="H15">
         <v>0</v>
       </c>
@@ -1309,9 +1511,11 @@
       <c r="J15">
         <v>0</v>
       </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
       <c r="L15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.238232746226</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1333,6 +1537,9 @@
       <c r="F16" t="s">
         <v>119</v>
       </c>
+      <c r="G16" t="s">
+        <v>161</v>
+      </c>
       <c r="H16">
         <v>1</v>
       </c>
@@ -1342,9 +1549,11 @@
       <c r="J16">
         <v>0</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
       <c r="L16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.281524724036</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1366,6 +1575,9 @@
       <c r="F17" t="s">
         <v>119</v>
       </c>
+      <c r="G17" t="s">
+        <v>140</v>
+      </c>
       <c r="H17">
         <v>9</v>
       </c>
@@ -1375,9 +1587,11 @@
       <c r="J17">
         <v>0</v>
       </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
       <c r="L17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.322636319353</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1399,6 +1613,9 @@
       <c r="F18" t="s">
         <v>117</v>
       </c>
+      <c r="G18" t="s">
+        <v>142</v>
+      </c>
       <c r="H18">
         <v>9</v>
       </c>
@@ -1408,9 +1625,11 @@
       <c r="J18">
         <v>0</v>
       </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
       <c r="L18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.332779608718</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1432,6 +1651,9 @@
       <c r="F19" t="s">
         <v>118</v>
       </c>
+      <c r="G19" t="s">
+        <v>152</v>
+      </c>
       <c r="H19">
         <v>1</v>
       </c>
@@ -1441,9 +1663,11 @@
       <c r="J19">
         <v>0</v>
       </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
       <c r="L19" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.372200663252</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1465,6 +1689,9 @@
       <c r="F20" t="s">
         <v>117</v>
       </c>
+      <c r="G20" t="s">
+        <v>143</v>
+      </c>
       <c r="H20">
         <v>7</v>
       </c>
@@ -1474,9 +1701,11 @@
       <c r="J20">
         <v>0</v>
       </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
       <c r="L20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.379662346291</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1498,6 +1727,9 @@
       <c r="F21" t="s">
         <v>117</v>
       </c>
+      <c r="G21" t="s">
+        <v>144</v>
+      </c>
       <c r="H21">
         <v>7</v>
       </c>
@@ -1507,9 +1739,11 @@
       <c r="J21">
         <v>0</v>
       </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
       <c r="L21" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.387551387255</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1531,6 +1765,9 @@
       <c r="F22" t="s">
         <v>118</v>
       </c>
+      <c r="G22" t="s">
+        <v>145</v>
+      </c>
       <c r="H22">
         <v>10</v>
       </c>
@@ -1540,9 +1777,11 @@
       <c r="J22">
         <v>0</v>
       </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
       <c r="L22" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.455635045611</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1564,6 +1803,9 @@
       <c r="F23" t="s">
         <v>117</v>
       </c>
+      <c r="G23" t="s">
+        <v>162</v>
+      </c>
       <c r="H23">
         <v>3</v>
       </c>
@@ -1573,9 +1815,11 @@
       <c r="J23">
         <v>0</v>
       </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
       <c r="L23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.51539491993</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1597,6 +1841,9 @@
       <c r="F24" t="s">
         <v>119</v>
       </c>
+      <c r="G24" t="s">
+        <v>155</v>
+      </c>
       <c r="H24">
         <v>9</v>
       </c>
@@ -1606,9 +1853,11 @@
       <c r="J24">
         <v>0</v>
       </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
       <c r="L24" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.544744543164</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1630,6 +1879,9 @@
       <c r="F25" t="s">
         <v>118</v>
       </c>
+      <c r="G25" t="s">
+        <v>160</v>
+      </c>
       <c r="H25">
         <v>4</v>
       </c>
@@ -1639,9 +1891,11 @@
       <c r="J25">
         <v>0</v>
       </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
       <c r="L25" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.569647729368</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1663,6 +1917,9 @@
       <c r="F26" t="s">
         <v>117</v>
       </c>
+      <c r="G26" t="s">
+        <v>166</v>
+      </c>
       <c r="H26">
         <v>3</v>
       </c>
@@ -1672,9 +1929,11 @@
       <c r="J26">
         <v>0</v>
       </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
       <c r="L26" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.598393264423</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1696,6 +1955,9 @@
       <c r="F27" t="s">
         <v>118</v>
       </c>
+      <c r="G27" t="s">
+        <v>167</v>
+      </c>
       <c r="H27">
         <v>4</v>
       </c>
@@ -1705,9 +1967,11 @@
       <c r="J27">
         <v>0</v>
       </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
       <c r="L27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.607357668749</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1729,6 +1993,9 @@
       <c r="F28" t="s">
         <v>117</v>
       </c>
+      <c r="G28" t="s">
+        <v>125</v>
+      </c>
       <c r="H28">
         <v>0</v>
       </c>
@@ -1738,9 +2005,11 @@
       <c r="J28">
         <v>0</v>
       </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
       <c r="L28" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.615151720027</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1762,6 +2031,9 @@
       <c r="F29" t="s">
         <v>118</v>
       </c>
+      <c r="G29" t="s">
+        <v>146</v>
+      </c>
       <c r="H29">
         <v>10</v>
       </c>
@@ -1771,9 +2043,11 @@
       <c r="J29">
         <v>0</v>
       </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
       <c r="L29" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.637815408038</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1795,6 +2069,9 @@
       <c r="F30" t="s">
         <v>117</v>
       </c>
+      <c r="G30" t="s">
+        <v>148</v>
+      </c>
       <c r="H30">
         <v>9</v>
       </c>
@@ -1804,9 +2081,11 @@
       <c r="J30">
         <v>1</v>
       </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
       <c r="L30" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.647760696258</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1828,6 +2107,9 @@
       <c r="F31" t="s">
         <v>117</v>
       </c>
+      <c r="G31" t="s">
+        <v>163</v>
+      </c>
       <c r="H31">
         <v>9</v>
       </c>
@@ -1835,11 +2117,13 @@
         <v>124</v>
       </c>
       <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
         <v>2</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.684361767519</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1861,65 +2145,75 @@
       <c r="F32" t="s">
         <v>117</v>
       </c>
+      <c r="G32" t="s">
+        <v>159</v>
+      </c>
       <c r="H32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
       <c r="L32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.685706018521</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
         <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E33" t="s">
         <v>117</v>
       </c>
       <c r="F33" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="G33" t="s">
+        <v>156</v>
       </c>
       <c r="H33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.686090951094</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E34" t="s">
         <v>117</v>
@@ -1927,8 +2221,11 @@
       <c r="F34" t="s">
         <v>118</v>
       </c>
+      <c r="G34" t="s">
+        <v>147</v>
+      </c>
       <c r="H34">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I34" t="s">
         <v>124</v>
@@ -1936,98 +2233,113 @@
       <c r="J34">
         <v>0</v>
       </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
       <c r="L34" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.713041139825</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
         <v>111</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F35" t="s">
         <v>118</v>
       </c>
+      <c r="G35" t="s">
+        <v>164</v>
+      </c>
       <c r="H35">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J35">
         <v>0</v>
       </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
       <c r="L35" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.714153954134</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="G36" t="s">
+        <v>165</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
       <c r="L36" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.735415707946</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F37" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="G37" t="s">
+        <v>150</v>
       </c>
       <c r="H37">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I37" t="s">
         <v>124</v>
@@ -2035,164 +2347,189 @@
       <c r="J37">
         <v>0</v>
       </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
       <c r="L37" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.757750973258</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F38" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="G38" t="s">
+        <v>151</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J38">
         <v>0</v>
       </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
       <c r="L38" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.76120808511</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F39" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="G39" t="s">
+        <v>168</v>
       </c>
       <c r="H39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J39">
         <v>0</v>
       </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
       <c r="L39" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.76606034502</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" t="s">
         <v>118</v>
       </c>
       <c r="F40" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="G40" t="s">
+        <v>169</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J40">
         <v>0</v>
       </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
       <c r="L40" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.866313337756</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E41" t="s">
         <v>118</v>
       </c>
       <c r="F41" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="G41" t="s">
+        <v>170</v>
       </c>
       <c r="H41">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J41">
         <v>0</v>
       </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
       <c r="L41" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.88017828008</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F42" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="G42" t="s">
+        <v>153</v>
       </c>
       <c r="H42">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I42" t="s">
         <v>124</v>
@@ -2200,111 +2537,412 @@
       <c r="J42">
         <v>0</v>
       </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
       <c r="L42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.897436756371</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F43" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="G43" t="s">
+        <v>172</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J43">
         <v>0</v>
       </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
       <c r="L43" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.905714783978</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E44" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F44" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="G44" t="s">
+        <v>139</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J44">
         <v>0</v>
       </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
       <c r="L44" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+        <v>45980.918957054455</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" t="s">
+        <v>117</v>
+      </c>
+      <c r="F45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45" t="s">
+        <v>128</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1">
+        <v>45980.944582879463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>55</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>59</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>113</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>110</v>
       </c>
-      <c r="E45" t="s">
-        <v>117</v>
-      </c>
-      <c r="F45" t="s">
-        <v>117</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45" t="s">
+      <c r="E46" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" t="s">
+        <v>171</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
         <v>125</v>
       </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="L45" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>45980.865575925927</v>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1">
+        <v>45980.96569405686</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC93F90-F40C-42AB-B047-CCC6F764A51E}">
+  <dimension ref="A1:A45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45979.989913523605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45980.004069368995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45980.054373367821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45980.062879867648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45980.065445785767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45980.068372531576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45980.096311333931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45980.140794824096</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45980.156893410371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45980.210053623603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45980.22066285491</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45980.223891000482</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45980.228297097412</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45980.238232746226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45980.281524724036</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45980.322636319353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45980.332779608718</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45980.372200663252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45980.379662346291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45980.387551387255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45980.455635045611</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45980.51539491993</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45980.544744543164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45980.569647729368</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45980.598393264423</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45980.607357668749</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45980.615151720027</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45980.637815408038</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45980.647760696258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45980.684361767519</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45980.686090951094</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45980.713041139825</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45980.714153954134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45980.735415707946</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45980.757750973258</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45980.76120808511</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45980.76606034502</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>45980.866313337756</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>45980.88017828008</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45980.897436756371</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45980.905714783978</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45980.918957054455</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45980.944582879463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>45980.96569405686</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A45">
+    <sortCondition ref="A2:A45"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Import of CSV to pgadmin
Change of file CSV file to eliminate trailing ;
creation of table in pgadmin
Import into pgadmin
</commit_message>
<xml_diff>
--- a/Audit Table.xlsx
+++ b/Audit Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VICTUS\Documents\GitHub\sql-quality-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC8F16-3B83-4D0C-B4DD-20491F23A9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10A26B1-EBC8-425F-9A92-23D7C6AE2C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3C1F016C-EBC1-4B48-98C7-798CC0259E45}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{3C1F016C-EBC1-4B48-98C7-798CC0259E45}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
@@ -38,42 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="173">
   <si>
-    <t>Audit_id</t>
-  </si>
-  <si>
-    <t>Auditor Name</t>
-  </si>
-  <si>
-    <t>Agent Name</t>
-  </si>
-  <si>
-    <t>Case ID</t>
-  </si>
-  <si>
-    <t>Case_type</t>
-  </si>
-  <si>
-    <t>Case_subtype</t>
-  </si>
-  <si>
-    <t>Error Description</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
-    <t>Audit_result</t>
-  </si>
-  <si>
-    <t>Was_reworked</t>
-  </si>
-  <si>
-    <t>Number of Reworks</t>
-  </si>
-  <si>
-    <t>Audit_time</t>
-  </si>
-  <si>
     <t>A-236551</t>
   </si>
   <si>
@@ -555,6 +519,42 @@
   </si>
   <si>
     <t>missing email</t>
+  </si>
+  <si>
+    <t>audit_id</t>
+  </si>
+  <si>
+    <t>auditor</t>
+  </si>
+  <si>
+    <t>agent</t>
+  </si>
+  <si>
+    <t>case_id</t>
+  </si>
+  <si>
+    <t>case_type</t>
+  </si>
+  <si>
+    <t>case_subtype</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>audit_result</t>
+  </si>
+  <si>
+    <t>was_reworked</t>
+  </si>
+  <si>
+    <t>rework_number</t>
+  </si>
+  <si>
+    <t>audit_time</t>
   </si>
 </sst>
 </file>
@@ -930,7 +930,7 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -949,69 +949,69 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>164</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H2">
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1025,31 +1025,31 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
         <v>119</v>
       </c>
-      <c r="F3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" t="s">
-        <v>131</v>
-      </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1063,31 +1063,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1101,31 +1101,31 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1139,31 +1139,31 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F6" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1177,31 +1177,31 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
         <v>113</v>
-      </c>
-      <c r="D7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" t="s">
-        <v>135</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>125</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1215,31 +1215,31 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="H8">
         <v>9</v>
       </c>
       <c r="I8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1253,31 +1253,31 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H9">
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1291,31 +1291,31 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G10" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="H10">
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1329,31 +1329,31 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1367,31 +1367,31 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="F12" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1405,31 +1405,31 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1443,31 +1443,31 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
         <v>113</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G14" t="s">
-        <v>157</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
-        <v>125</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1481,31 +1481,31 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F15" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G15" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1519,31 +1519,31 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F16" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G16" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1557,31 +1557,31 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="H17">
         <v>9</v>
       </c>
       <c r="I17" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1595,31 +1595,31 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F18" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H18">
         <v>9</v>
       </c>
       <c r="I18" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1633,31 +1633,31 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G19" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1671,31 +1671,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G20" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="H20">
         <v>7</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1709,31 +1709,31 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G21" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="H21">
         <v>7</v>
       </c>
       <c r="I21" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1747,31 +1747,31 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G22" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1785,31 +1785,31 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F23" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="H23">
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -1823,31 +1823,31 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G24" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="H24">
         <v>9</v>
       </c>
       <c r="I24" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1861,31 +1861,31 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G25" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="H25">
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1899,31 +1899,31 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F26" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G26" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="H26">
         <v>3</v>
       </c>
       <c r="I26" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1937,31 +1937,31 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F27" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G27" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="H27">
         <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1975,31 +1975,31 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F28" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G28" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -2013,31 +2013,31 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F29" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="H29">
         <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -2051,31 +2051,31 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F30" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G30" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="H30">
         <v>9</v>
       </c>
       <c r="I30" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2089,31 +2089,31 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F31" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G31" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="H31">
         <v>9</v>
       </c>
       <c r="I31" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2127,31 +2127,31 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" t="s">
         <v>57</v>
       </c>
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F32" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G32" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="H32">
         <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -2165,31 +2165,31 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
         <v>57</v>
       </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E33" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G33" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2203,31 +2203,31 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="H34">
         <v>5</v>
       </c>
       <c r="I34" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -2241,31 +2241,31 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="H35">
         <v>10</v>
       </c>
       <c r="I35" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -2279,31 +2279,31 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F36" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G36" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2317,31 +2317,31 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D37" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F37" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G37" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -2355,31 +2355,31 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F38" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G38" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="H38">
         <v>8</v>
       </c>
       <c r="I38" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2393,31 +2393,31 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F39" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G39" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2431,31 +2431,31 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F40" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G40" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="H40">
         <v>8</v>
       </c>
       <c r="I40" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2469,31 +2469,31 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E41" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F41" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G41" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2507,31 +2507,31 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D42" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E42" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F42" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G42" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="H42">
         <v>10</v>
       </c>
       <c r="I42" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -2545,31 +2545,31 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" t="s">
         <v>107</v>
       </c>
-      <c r="E43" t="s">
-        <v>119</v>
-      </c>
       <c r="F43" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G43" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="H43">
         <v>5</v>
       </c>
       <c r="I43" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2583,31 +2583,31 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D44" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F44" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G44" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -2621,31 +2621,31 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E45" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F45" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G45" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -2659,31 +2659,31 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" t="s">
+        <v>105</v>
+      </c>
+      <c r="F46" t="s">
+        <v>105</v>
+      </c>
+      <c r="G46" t="s">
+        <v>159</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
         <v>113</v>
-      </c>
-      <c r="D46" t="s">
-        <v>110</v>
-      </c>
-      <c r="E46" t="s">
-        <v>117</v>
-      </c>
-      <c r="F46" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" t="s">
-        <v>171</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46" t="s">
-        <v>125</v>
       </c>
       <c r="J46">
         <v>0</v>

</xml_diff>